<commit_message>
Add convenience projection strings
</commit_message>
<xml_diff>
--- a/inst/extdata/gis/crs_proj.xlsx
+++ b/inst/extdata/gis/crs_proj.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pascalburkhard/Dropbox/Work/Geography/Visualization/R/Packages/geotools/inst/extdata/gis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{30EEB6E6-CCB0-0B4F-8504-35FF8EBABEE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7855CFB8-DE2E-DC4D-BCB4-503EDEA9A1C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4660" yWindow="4420" windowWidth="27640" windowHeight="16940" xr2:uid="{4AF92194-DDBF-3343-BE0F-307CCB295B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>crs</t>
   </si>
@@ -46,6 +46,42 @@
   </si>
   <si>
     <t>+proj=eqearth +lon_0=0 +x_0=0 +y_0=0 +datum=WGS84 +units=m +no_defs</t>
+  </si>
+  <si>
+    <t>+proj=wintri +datum=WGS84 +no_defs +over</t>
+  </si>
+  <si>
+    <t>wintri</t>
+  </si>
+  <si>
+    <t>robinson</t>
+  </si>
+  <si>
+    <t>+proj=robin +lat_0=0 +lon_0=0 +x0=0 +y0=0</t>
+  </si>
+  <si>
+    <t>equirec</t>
+  </si>
+  <si>
+    <t>+proj=longlat +ellps=WGS84 +datum=WGS84 +no_defs</t>
+  </si>
+  <si>
+    <t>gallpeters</t>
+  </si>
+  <si>
+    <t>+proj=cea +lon_0=0 +lat_ts=45 +x_0=0 +y_0=0 +ellps=WGS84 +units=m +no_defs</t>
+  </si>
+  <si>
+    <t>hobodyer</t>
+  </si>
+  <si>
+    <t>+proj=cea +lat_ts=37.5</t>
+  </si>
+  <si>
+    <t>goode</t>
+  </si>
+  <si>
+    <t>+proj=igh</t>
   </si>
 </sst>
 </file>
@@ -398,15 +434,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150750DA-0E9C-D942-94EA-50CA415CE4DB}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="65.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="109.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -425,7 +461,58 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B8">
+    <sortCondition ref="A2:A8"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add mercator convenience projection string
</commit_message>
<xml_diff>
--- a/inst/extdata/gis/crs_proj.xlsx
+++ b/inst/extdata/gis/crs_proj.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pascalburkhard/Dropbox/Work/Geography/Visualization/R/Packages/geotools/inst/extdata/gis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7855CFB8-DE2E-DC4D-BCB4-503EDEA9A1C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9094B981-8357-F046-AD82-9C4FC1BB3C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4660" yWindow="4420" windowWidth="27640" windowHeight="16940" xr2:uid="{4AF92194-DDBF-3343-BE0F-307CCB295B18}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>crs</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>+proj=igh</t>
+  </si>
+  <si>
+    <t>mercator</t>
+  </si>
+  <si>
+    <t>+proj=merc +lon_0=0 +k=1 +x_0=0 +y_0=0 +ellps=WGS84 +datum=WGS84 +units=m +no_defs"</t>
   </si>
 </sst>
 </file>
@@ -434,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150750DA-0E9C-D942-94EA-50CA415CE4DB}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -495,23 +501,31 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B8">
-    <sortCondition ref="A2:A8"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B9">
+    <sortCondition ref="A2:A9"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix equirectangular projection string
</commit_message>
<xml_diff>
--- a/inst/extdata/gis/crs_proj.xlsx
+++ b/inst/extdata/gis/crs_proj.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pascalburkhard/Dropbox/Work/Geography/Visualization/R/Packages/geotools/inst/extdata/gis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9094B981-8357-F046-AD82-9C4FC1BB3C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E387F7-B616-1049-9EA0-D434B580697B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4660" yWindow="4420" windowWidth="27640" windowHeight="16940" xr2:uid="{4AF92194-DDBF-3343-BE0F-307CCB295B18}"/>
+    <workbookView xWindow="1160" yWindow="1060" windowWidth="27640" windowHeight="16940" xr2:uid="{4AF92194-DDBF-3343-BE0F-307CCB295B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,9 +63,6 @@
     <t>equirec</t>
   </si>
   <si>
-    <t>+proj=longlat +ellps=WGS84 +datum=WGS84 +no_defs</t>
-  </si>
-  <si>
     <t>gallpeters</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>+proj=merc +lon_0=0 +k=1 +x_0=0 +y_0=0 +ellps=WGS84 +datum=WGS84 +units=m +no_defs"</t>
+  </si>
+  <si>
+    <t>+proj=eqc</t>
   </si>
 </sst>
 </file>
@@ -443,7 +443,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -472,39 +472,39 @@
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>